<commit_message>
Updated the script to include status report and error handling
</commit_message>
<xml_diff>
--- a/data/Input.xlsx
+++ b/data/Input.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gaurav K\Python\Python_Examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gaurav K\GIT Repo\configure-teams-access\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0754AA-CBA2-436D-BBC9-EC029AF5E686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9442BCB-8602-4B5B-9ED4-5696EEBAA8F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{6CD408BF-E6BB-4C5F-A8FA-DFF3C7943EA0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>Repository Name</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>ThirdGitHubRepo</t>
+  </si>
+  <si>
+    <t>ScondGithubRepo-TeamRead</t>
   </si>
 </sst>
 </file>
@@ -424,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FF14CA6-86BC-4A3F-B845-F621FEBF7E7C}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -494,13 +497,13 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -508,10 +511,10 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -519,9 +522,20 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated the Input file
</commit_message>
<xml_diff>
--- a/data/Input.xlsx
+++ b/data/Input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gaurav K\GIT Repo\configure-teams-access\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9442BCB-8602-4B5B-9ED4-5696EEBAA8F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF86DB66-2920-4A8F-9403-EEA8E2F80867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{6CD408BF-E6BB-4C5F-A8FA-DFF3C7943EA0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>Repository Name</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>ScondGithubRepo-TeamRead</t>
+  </si>
+  <si>
+    <t>Hfdlfsfdsf</t>
   </si>
 </sst>
 </file>
@@ -427,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FF14CA6-86BC-4A3F-B845-F621FEBF7E7C}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -539,6 +542,17 @@
         <v>3</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>